<commit_message>
Implemented the basics following Unity's official tutorial
</commit_message>
<xml_diff>
--- a/Documentation/Workhours.xlsx
+++ b/Documentation/Workhours.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\SimpleAuto-Unity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\SimpleAuto-Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C81FE0E-11E5-4E64-91C0-A6604DF6D970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDCDFA3-214E-4082-B0E3-BD75067C33EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>From</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>Task description</t>
+  </si>
+  <si>
+    <t>Unity WheelCollider documentation</t>
+  </si>
+  <si>
+    <t>Unity WheelCollider tutorial</t>
   </si>
 </sst>
 </file>
@@ -114,11 +120,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D2"/>
+  <dimension ref="B1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,6 +429,39 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="4">
+        <v>0.30902777777777779</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.31597222222222221</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="4">
+        <v>0.31597222222222221</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Basic driving with animated gear shift, clutch and steeringwheel
</commit_message>
<xml_diff>
--- a/Documentation/Workhours.xlsx
+++ b/Documentation/Workhours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\SimpleAuto-Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDCDFA3-214E-4082-B0E3-BD75067C33EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA992DB1-2717-4784-822C-61F5B9E2BD0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>From</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Unity WheelCollider tutorial</t>
+  </si>
+  <si>
+    <t>Dashboard modelling with Probuilder</t>
+  </si>
+  <si>
+    <t>Pedals and gearbox</t>
   </si>
 </sst>
 </file>
@@ -406,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D5"/>
+  <dimension ref="B1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,6 +468,39 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.46875</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
End of the day
</commit_message>
<xml_diff>
--- a/Documentation/Workhours.xlsx
+++ b/Documentation/Workhours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\SimpleAuto-Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA992DB1-2717-4784-822C-61F5B9E2BD0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF059CC7-2958-4043-84B2-1020D91D9592}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>From</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Pedals and gearbox</t>
+  </si>
+  <si>
+    <t>Video</t>
   </si>
 </sst>
 </file>
@@ -126,12 +129,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D8"/>
+  <dimension ref="B1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,80 +442,91 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="4">
+      <c r="B3" s="1">
         <v>0.30902777777777779</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="1">
         <v>0.31597222222222221</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="4">
+      <c r="B4" s="1">
         <v>0.31597222222222221</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="4">
+      <c r="B5" s="1">
         <v>0.34027777777777773</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="1">
         <v>0.375</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="4">
+      <c r="B6" s="1">
         <v>0.375</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="1">
         <v>0.3888888888888889</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="4">
+      <c r="B7" s="1">
         <v>0.3923611111111111</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="4">
+      <c r="B8" s="1">
         <v>0.43055555555555558</v>
       </c>
-      <c r="C8" s="4">
-        <v>0.46875</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C8" s="1">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inverted steering bug fixed
</commit_message>
<xml_diff>
--- a/Documentation/Workhours.xlsx
+++ b/Documentation/Workhours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\SimpleAuto-Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF059CC7-2958-4043-84B2-1020D91D9592}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9050006C-1E74-4C81-B99E-4F3D5003C55F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>From</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>Video</t>
+  </si>
+  <si>
+    <t>Trying to figure out the cause of inverted steeringwheel rotation</t>
+  </si>
+  <si>
+    <t>Researching IK</t>
+  </si>
+  <si>
+    <t>Importing rigged 3D character</t>
   </si>
 </sst>
 </file>
@@ -129,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -137,17 +146,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -429,26 +444,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D9"/>
+  <dimension ref="B1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="36.7109375" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="5"/>
+    <col min="4" max="4" width="55" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -519,14 +535,56 @@
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
+      <c r="B9" s="3">
         <v>0.47222222222222227</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="3">
         <v>0.4861111111111111</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved car visuals and camera.
</commit_message>
<xml_diff>
--- a/Documentation/Workhours.xlsx
+++ b/Documentation/Workhours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\SimpleAuto-Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9050006C-1E74-4C81-B99E-4F3D5003C55F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0233CEEC-BC0D-402F-84F5-1BC1F786CADB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>From</t>
   </si>
@@ -57,7 +57,31 @@
     <t>Researching IK</t>
   </si>
   <si>
-    <t>Importing rigged 3D character</t>
+    <t>Importing low poly asset pack for character and car visuals.</t>
+  </si>
+  <si>
+    <t>~12:30</t>
+  </si>
+  <si>
+    <t>Modelling missing or unmovable props (steering wheel, handbrake, pedals, gearshift)</t>
+  </si>
+  <si>
+    <t>Importing the new assets, fixing rotation and scale problems. There are some problems with the pedals normals.</t>
+  </si>
+  <si>
+    <t>Realized, that i was editing different files, then what I exported to Unity, cause I made a backup to different folders…</t>
+  </si>
+  <si>
+    <t>Editing the real files… Still, there is some bug with the import, the rotation is off, but it does not really matter.</t>
+  </si>
+  <si>
+    <t>Finished the the car visuals.</t>
+  </si>
+  <si>
+    <t>Importing and stripping down my camera controller from another project. Added different camera positions with limited rotation.</t>
+  </si>
+  <si>
+    <t>Added headlights.</t>
   </si>
 </sst>
 </file>
@@ -138,20 +162,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -161,8 +179,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -444,24 +471,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D14"/>
+  <dimension ref="B1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="9.140625" style="5"/>
-    <col min="4" max="4" width="55" style="5" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="58.28515625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -475,7 +502,7 @@
       <c r="C3" s="1">
         <v>0.31597222222222221</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -486,7 +513,7 @@
       <c r="C4" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -497,7 +524,7 @@
       <c r="C5" s="1">
         <v>0.375</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -508,7 +535,7 @@
       <c r="C6" s="1">
         <v>0.3888888888888889</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="6" t="s">
         <v>5</v>
       </c>
     </row>
@@ -519,7 +546,7 @@
       <c r="C7" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -530,27 +557,27 @@
       <c r="C8" s="1">
         <v>0.47222222222222227</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>0.47222222222222227</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>0.4861111111111111</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="8" t="s">
@@ -558,33 +585,113 @@
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>0.48958333333333331</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>0.5</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>0.5</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>0.50694444444444442</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>0.50694444444444442</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited the car asset, assigned materials, fixed character rig.
</commit_message>
<xml_diff>
--- a/Documentation/Workhours.xlsx
+++ b/Documentation/Workhours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\SimpleAuto-Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0233CEEC-BC0D-402F-84F5-1BC1F786CADB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB167DB5-2C24-46D5-89F7-B8EFCDFD0107}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>From</t>
   </si>
@@ -82,6 +82,21 @@
   </si>
   <si>
     <t>Added headlights.</t>
+  </si>
+  <si>
+    <t>Character, tried to create basic sit animation inside Unity.</t>
+  </si>
+  <si>
+    <t>Assigned materials to the car in blender, fixed the import issues.</t>
+  </si>
+  <si>
+    <t>Animating character in Blender.</t>
+  </si>
+  <si>
+    <t>Fixing up bone names in Blender…</t>
+  </si>
+  <si>
+    <t>Character finally proparly imported…</t>
   </si>
 </sst>
 </file>
@@ -471,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D21"/>
+  <dimension ref="B1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,6 +709,61 @@
         <v>18</v>
       </c>
     </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="2">
+        <v>0.76736111111111116</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.77569444444444446</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="2">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.79583333333333339</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <v>0.79583333333333339</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Basic avatar with hand IK
</commit_message>
<xml_diff>
--- a/Documentation/Workhours.xlsx
+++ b/Documentation/Workhours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\SimpleAuto-Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB167DB5-2C24-46D5-89F7-B8EFCDFD0107}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17065526-DAF6-466E-9528-F1F3D21A078B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>From</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Character finally proparly imported…</t>
+  </si>
+  <si>
+    <t>Coding AvatarAnimationController (IK)</t>
   </si>
 </sst>
 </file>
@@ -486,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D26"/>
+  <dimension ref="B1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,6 +767,17 @@
         <v>23</v>
       </c>
     </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
+        <v>0.81944444444444453</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Car prefab updated, Grab blend tree added.
</commit_message>
<xml_diff>
--- a/Documentation/Workhours.xlsx
+++ b/Documentation/Workhours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\SimpleAuto-Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17065526-DAF6-466E-9528-F1F3D21A078B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E49A33-45FE-4591-B4ED-2DADBE417DE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>From</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>Coding AvatarAnimationController (IK)</t>
+  </si>
+  <si>
+    <t>Updating the prefab to the new car.</t>
+  </si>
+  <si>
+    <t>Reseraching Animation layers for the hands.</t>
+  </si>
+  <si>
+    <t>Importing timer from my other project.</t>
   </si>
 </sst>
 </file>
@@ -489,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D27"/>
+  <dimension ref="B1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,6 +787,36 @@
         <v>24</v>
       </c>
     </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>0.84375</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.88194444444444453</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>0.88194444444444453</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Leg Ik, Bug found with curent IK system
</commit_message>
<xml_diff>
--- a/Documentation/Workhours.xlsx
+++ b/Documentation/Workhours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\SimpleAuto-Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF211F7-8C5C-4742-BC90-08E5046FB8B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25C8641-D592-4B5C-9F4A-14B7E0CD0E2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>From</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Finally figured IK interpolation out… :D</t>
+  </si>
+  <si>
+    <t>There are some bugs with the IK interpolation while movin.</t>
   </si>
 </sst>
 </file>
@@ -507,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D33"/>
+  <dimension ref="B1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,6 +865,17 @@
         <v>30</v>
       </c>
     </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
IKAnimator position lerp finished
</commit_message>
<xml_diff>
--- a/Documentation/Workhours.xlsx
+++ b/Documentation/Workhours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\SimpleAuto-Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25C8641-D592-4B5C-9F4A-14B7E0CD0E2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91DE714-16C5-4074-B7C3-7950CB35B95D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>From</t>
   </si>
@@ -121,6 +121,24 @@
   </si>
   <si>
     <t>There are some bugs with the IK interpolation while movin.</t>
+  </si>
+  <si>
+    <t>Solved IK bug.</t>
+  </si>
+  <si>
+    <t>Setting up nicer IK positions.</t>
+  </si>
+  <si>
+    <t>Lerping the rotation sometimes results in the Ik taking the longer rotation. Searching for a fix.</t>
+  </si>
+  <si>
+    <t>Fixing skipping if the goal is changed mid transition.</t>
+  </si>
+  <si>
+    <t>Make it possible to Deatach the ik from the goal, so it will not teleport after the goal, just treat it as a new goal.</t>
+  </si>
+  <si>
+    <t>Ik working correctly for every limb, except the rotation lerp.</t>
   </si>
 </sst>
 </file>
@@ -510,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D34"/>
+  <dimension ref="B1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,6 +894,72 @@
         <v>31</v>
       </c>
     </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="2">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.53125</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="2">
+        <v>0.5493055555555556</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="2">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="2">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.78819444444444453</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Clock MVVM - Background and Pointer finished
</commit_message>
<xml_diff>
--- a/Documentation/Workhours.xlsx
+++ b/Documentation/Workhours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\SimpleAuto-Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9C445B-8FC0-4C9A-84BF-A882F30A6BA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759AED3D-39A2-4D43-BF1D-247189DD63F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>From</t>
   </si>
@@ -196,6 +196,27 @@
   </si>
   <si>
     <t>Set up prefab to work with new script. When both pedal pressed, the rotation is calculated now from the brake to the gas.</t>
+  </si>
+  <si>
+    <t>Made basic sprites for GUI in AseSprite.</t>
+  </si>
+  <si>
+    <t>Started to plan out Gui architechture.</t>
+  </si>
+  <si>
+    <t>Marks half finished, Background finished.</t>
+  </si>
+  <si>
+    <t>Working on implementing MVVM for Clock GUI.</t>
+  </si>
+  <si>
+    <t>ClockGui finished, except the markings.</t>
+  </si>
+  <si>
+    <t>Creating class to test the visuals.</t>
+  </si>
+  <si>
+    <t>Finished debuging…</t>
   </si>
 </sst>
 </file>
@@ -672,26 +693,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -973,10 +994,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,10 +1024,10 @@
       <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="50"/>
+      <c r="G2" s="55"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="11">
@@ -1113,7 +1134,7 @@
       <c r="F9" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="55"/>
+      <c r="G9" s="53"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1219,13 +1240,13 @@
       </c>
     </row>
     <row r="20" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B20" s="52">
+      <c r="B20" s="50">
         <v>0.61111111111111105</v>
       </c>
-      <c r="C20" s="53">
+      <c r="C20" s="51">
         <v>0.67361111111111116</v>
       </c>
-      <c r="D20" s="54" t="s">
+      <c r="D20" s="52" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1469,10 +1490,10 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="51">
+      <c r="B43" s="49">
         <v>0.8125</v>
       </c>
-      <c r="C43" s="51">
+      <c r="C43" s="49">
         <v>0.82638888888888884</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -1480,10 +1501,10 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B44" s="51">
+      <c r="B44" s="49">
         <v>0.82638888888888884</v>
       </c>
-      <c r="C44" s="51">
+      <c r="C44" s="49">
         <v>0.84027777777777779</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -1491,10 +1512,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="51">
+      <c r="B45" s="49">
         <v>0.86111111111111116</v>
       </c>
-      <c r="C45" s="51">
+      <c r="C45" s="49">
         <v>0.84375</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1517,10 +1538,10 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B48" s="51">
+      <c r="B48" s="49">
         <v>0.42708333333333331</v>
       </c>
-      <c r="C48" s="51">
+      <c r="C48" s="49">
         <v>0.4513888888888889</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -1528,10 +1549,10 @@
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="51">
+      <c r="B49" s="49">
         <v>0.49652777777777773</v>
       </c>
-      <c r="C49" s="51">
+      <c r="C49" s="49">
         <v>0.52777777777777779</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -1539,14 +1560,91 @@
       </c>
     </row>
     <row r="50" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B50" s="51">
+      <c r="B50" s="49">
         <v>0.52777777777777779</v>
       </c>
-      <c r="C50" s="51">
+      <c r="C50" s="49">
         <v>0.53749999999999998</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="49">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="C51" s="49">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="49">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="C52" s="49">
+        <v>0.625</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="49">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="C53" s="49">
+        <v>0.6875</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="49">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="C54" s="49">
+        <v>0.82986111111111116</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="49">
+        <v>0.82986111111111116</v>
+      </c>
+      <c r="C55" s="49">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="49">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C56" s="49">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="49">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="C57" s="49">
+        <v>0.53125</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ClockView - Mark placment.
</commit_message>
<xml_diff>
--- a/Documentation/Workhours.xlsx
+++ b/Documentation/Workhours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\SimpleAuto-Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759AED3D-39A2-4D43-BF1D-247189DD63F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BCC908-58EE-44C0-83C4-23C7C2B86987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>From</t>
   </si>
@@ -217,6 +217,21 @@
   </si>
   <si>
     <t>Finished debuging…</t>
+  </si>
+  <si>
+    <t>Day 5</t>
+  </si>
+  <si>
+    <t>Moved view settings to ClockViewStyle, implemented mark placement and ClockMarkView.</t>
+  </si>
+  <si>
+    <t>Update test script for the new features.</t>
+  </si>
+  <si>
+    <t>Debug mark placement. Marks almost placed correctly, right distance, but mirrored compared to the face.</t>
+  </si>
+  <si>
+    <t>I think the problem is in the face, not the marks.</t>
   </si>
 </sst>
 </file>
@@ -994,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1548,7 +1563,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" s="49">
         <v>0.49652777777777773</v>
       </c>
@@ -1559,7 +1574,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B50" s="49">
         <v>0.52777777777777779</v>
       </c>
@@ -1570,7 +1585,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" s="49">
         <v>0.55208333333333337</v>
       </c>
@@ -1581,7 +1596,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="49">
         <v>0.61111111111111105</v>
       </c>
@@ -1592,7 +1607,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" s="49">
         <v>0.63541666666666663</v>
       </c>
@@ -1603,7 +1618,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" s="49">
         <v>0.72222222222222221</v>
       </c>
@@ -1614,7 +1629,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" s="49">
         <v>0.82986111111111116</v>
       </c>
@@ -1625,7 +1640,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" s="49">
         <v>0.89583333333333337</v>
       </c>
@@ -1636,15 +1651,71 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" s="49">
         <v>0.90972222222222221</v>
       </c>
       <c r="C57" s="49">
-        <v>0.53125</v>
+        <v>1.03125</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" s="48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B60" s="49">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C60" s="49">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="49">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="C61" s="49">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B62" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="C62" s="49">
+        <v>0.5229166666666667</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="49">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ClockViewModel - New tweakable features added
</commit_message>
<xml_diff>
--- a/Documentation/Workhours.xlsx
+++ b/Documentation/Workhours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\SimpleAuto-Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E418F1B-EB51-446E-96A3-A2279BBF5C65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1639B923-C6DA-4C3A-8333-372740072258}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="86">
   <si>
     <t>From</t>
   </si>
@@ -283,6 +283,12 @@
   </si>
   <si>
     <t>Implement configurable text placement, text rrotationOffset.</t>
+  </si>
+  <si>
+    <t>Debugging RimExtreme value.</t>
+  </si>
+  <si>
+    <t>All known bugs fixed, extra features added for tweaking.</t>
   </si>
 </sst>
 </file>
@@ -950,16 +956,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1242,10 +1248,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD87"/>
+  <dimension ref="A1:XFD89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,10 +1282,10 @@
       <c r="E2" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="80" t="s">
+      <c r="G2" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="81"/>
+      <c r="H2" s="83"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="10">
@@ -18696,10 +18702,10 @@
       <c r="B73" s="45">
         <v>0.97222222222222221</v>
       </c>
-      <c r="C73" s="82">
+      <c r="C73" s="80">
         <v>0.51388888888888895</v>
       </c>
-      <c r="E73" s="83">
+      <c r="E73" s="81">
         <f>C73-B73</f>
         <v>-0.45833333333333326</v>
       </c>
@@ -18839,6 +18845,28 @@
       </c>
       <c r="D87" s="1" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="45">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C88" s="45">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="45">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="C89" s="45">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new ClockStyles-s, fixed some bug, added some new options
</commit_message>
<xml_diff>
--- a/Documentation/Workhours.xlsx
+++ b/Documentation/Workhours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\SimpleAuto-Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1639B923-C6DA-4C3A-8333-372740072258}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D223257D-CB02-49AA-97C7-45F9C2BDBB9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
   <si>
     <t>From</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>All known bugs fixed, extra features added for tweaking.</t>
+  </si>
+  <si>
+    <t>Tweaking visuals, creating sprites, fixing bugs.</t>
   </si>
 </sst>
 </file>
@@ -1248,10 +1251,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD89"/>
+  <dimension ref="A1:XFD90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18869,6 +18872,17 @@
         <v>85</v>
       </c>
     </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="45">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C90" s="45">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G2:H2"/>

</xml_diff>